<commit_message>
Changes made and imported pillow lib
</commit_message>
<xml_diff>
--- a/Source/invoice template.xlsx
+++ b/Source/invoice template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPankaj\Sample Superstore Invoices project\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4203599B-F462-4CDA-B132-A1BD586C1AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E0D69A-ACAF-451E-9CA4-03DFF18019DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0715FA10-8D01-45E7-82DD-727F4E460AB6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Order ID</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>This is a system generated receipt, hence signature not required.</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Sales</t>
   </si>
 </sst>
 </file>
@@ -87,14 +105,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="35"/>
       <color theme="8" tint="-0.499984740745262"/>
@@ -109,8 +119,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +146,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,9 +160,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -161,25 +199,26 @@
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -206,7 +245,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:colOff>220980</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
@@ -547,18 +586,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3455C4-A3FC-4571-B999-EF0BAD12297D}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11.21875" customWidth="1"/>
     <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
@@ -601,17 +645,17 @@
     <row r="3" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="14"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -620,15 +664,15 @@
     <row r="4" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="14"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -637,15 +681,15 @@
     <row r="5" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="14"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -654,7 +698,7 @@
     <row r="6" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="14"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -840,12 +884,24 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="C16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -857,12 +913,12 @@
     <row r="17" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -874,12 +930,12 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -891,12 +947,12 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -908,12 +964,12 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -925,12 +981,12 @@
     <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -942,12 +998,12 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -959,12 +1015,12 @@
     <row r="23" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -973,15 +1029,15 @@
       <c r="N23" s="2"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -990,15 +1046,15 @@
       <c r="N24" s="2"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1007,17 +1063,15 @@
       <c r="N25" s="2"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1026,17 +1080,15 @@
       <c r="N26" s="2"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1045,15 +1097,15 @@
       <c r="N27" s="2"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1062,22 +1114,128 @@
       <c r="N28" s="2"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
       <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Changes made in code, uninstalled pillow lib.
</commit_message>
<xml_diff>
--- a/Source/invoice template.xlsx
+++ b/Source/invoice template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPankaj\Sample Superstore Invoices project\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E0D69A-ACAF-451E-9CA4-03DFF18019DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4C037D-E19F-4B7C-BE2A-1B18CC465C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0715FA10-8D01-45E7-82DD-727F4E460AB6}"/>
   </bookViews>
@@ -209,13 +209,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3455C4-A3FC-4571-B999-EF0BAD12297D}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,17 +645,17 @@
     <row r="3" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="13"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="2"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -664,15 +664,15 @@
     <row r="4" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="2"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -681,15 +681,15 @@
     <row r="5" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="13"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="2"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -698,7 +698,7 @@
     <row r="6" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="13"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -915,10 +915,10 @@
       <c r="B17" s="2"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="14"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -930,12 +930,12 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -947,12 +947,12 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -964,12 +964,12 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -981,12 +981,12 @@
     <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -998,12 +998,12 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1015,12 +1015,12 @@
     <row r="23" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1032,12 +1032,12 @@
     <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1049,12 +1049,12 @@
     <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1066,12 +1066,12 @@
     <row r="26" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1083,12 +1083,12 @@
     <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1100,12 +1100,12 @@
     <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1117,12 +1117,12 @@
     <row r="29" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1134,12 +1134,12 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1151,12 +1151,12 @@
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>

</xml_diff>